<commit_message>
feat: add AI processing steps display and cleanup temp files
</commit_message>
<xml_diff>
--- a/checked_data.xlsx
+++ b/checked_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data_agent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25525F5A-3F44-416D-8CA1-BEDEF7271B18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F905F47C-B2F1-42BC-9BDE-96AC67ED0E03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1450" yWindow="1300" windowWidth="16520" windowHeight="11170" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7040" yWindow="2900" windowWidth="16520" windowHeight="11170" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="用户表" sheetId="1" r:id="rId1"/>
@@ -1466,13 +1466,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:L9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="31.54296875" customWidth="1"/>
+    <col min="5" max="5" width="12.26953125" customWidth="1"/>
+    <col min="6" max="6" width="16.1796875" customWidth="1"/>
     <col min="7" max="7" width="12.36328125" customWidth="1"/>
     <col min="8" max="8" width="14.453125" customWidth="1"/>
     <col min="9" max="9" width="8.36328125" customWidth="1"/>
@@ -2196,7 +2198,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -2389,6 +2391,7 @@
     <col min="2" max="2" width="11.08984375" customWidth="1"/>
     <col min="4" max="4" width="17.36328125" customWidth="1"/>
     <col min="8" max="8" width="18.54296875" customWidth="1"/>
+    <col min="10" max="10" width="17.7265625" customWidth="1"/>
     <col min="11" max="11" width="37.08984375" customWidth="1"/>
     <col min="12" max="12" width="29" customWidth="1"/>
   </cols>
@@ -3024,8 +3027,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>

</xml_diff>